<commit_message>
Fixed a bug issue
</commit_message>
<xml_diff>
--- a/complete reports/Comparing Filters.xlsx
+++ b/complete reports/Comparing Filters.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\School Work\CSC\CSC2002S\Assignments\CHNTIN004_CSC2002S_Assignment_1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\School Work\CSC\CSC2002S\Assignments\CHNTIN004_CSC2002S_Assignment_1\complete reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Comparing Filters" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -36,10 +36,10 @@
     <t>warm up  of 10 runs</t>
   </si>
   <si>
-    <t>averaged over 20 runs</t>
+    <t>4 cores (my PC)</t>
   </si>
   <si>
-    <t>4 cores (my PC)</t>
+    <t>averaged over 50 runs</t>
   </si>
 </sst>
 </file>
@@ -802,11 +802,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1768180464"/>
-        <c:axId val="1768182096"/>
+        <c:axId val="202581776"/>
+        <c:axId val="202579600"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1768180464"/>
+        <c:axId val="202581776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -848,7 +848,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1768182096"/>
+        <c:crossAx val="202579600"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -856,7 +856,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1768182096"/>
+        <c:axId val="202579600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -907,7 +907,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1768180464"/>
+        <c:crossAx val="202581776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1831,8 +1831,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1866,8 +1866,12 @@
       <c r="C2">
         <v>0.112873354</v>
       </c>
+      <c r="D2">
+        <f>C2/B2</f>
+        <v>2.5409646392065746</v>
+      </c>
       <c r="E2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1880,6 +1884,10 @@
       <c r="C3">
         <v>0.14590594300000001</v>
       </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D11" si="0">C3/B3</f>
+        <v>2.7249292765850242</v>
+      </c>
       <c r="E3" t="s">
         <v>4</v>
       </c>
@@ -1894,8 +1902,12 @@
       <c r="C4">
         <v>0.18816943699999999</v>
       </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>2.8572327897787377</v>
+      </c>
       <c r="E4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1908,6 +1920,10 @@
       <c r="C5">
         <v>0.24175914800000001</v>
       </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>3.0937926420148094</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -1919,6 +1935,10 @@
       <c r="C6">
         <v>0.30965748199999998</v>
       </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>3.4014006973444393</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -1930,6 +1950,10 @@
       <c r="C7">
         <v>0.39343784199999998</v>
       </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>3.4381770018603519</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -1941,6 +1965,10 @@
       <c r="C8">
         <v>0.48670976999999999</v>
       </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>3.6409145147338875</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
@@ -1952,6 +1980,10 @@
       <c r="C9">
         <v>0.59994905600000004</v>
       </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>3.7236465845374398</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -1963,6 +1995,10 @@
       <c r="C10">
         <v>0.70783379700000004</v>
       </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>3.8239819936324175</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -1973,6 +2009,10 @@
       </c>
       <c r="C11">
         <v>0.82933537000000002</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>3.8610488680162676</v>
       </c>
     </row>
   </sheetData>

</xml_diff>